<commit_message>
Auditoria al monitoreo de actividades del 1 al 8 abril, 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Calidad/Checklist_organizacional_externo_160408.xlsx
+++ b/Proyectos/2016/Calidad/Checklist_organizacional_externo_160408.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="126">
   <si>
     <t>DATOS GENERALES</t>
   </si>
@@ -397,6 +397,12 @@
   <si>
     <t>Al no haber sido realizada la tarea no cuenta con registro de tiempo.</t>
   </si>
+  <si>
+    <t>SOS Software</t>
+  </si>
+  <si>
+    <t>Selenne Chávez</t>
+  </si>
 </sst>
 </file>
 
@@ -693,46 +699,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -875,8 +843,49 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1228,21 +1237,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK43"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="15"/>
-    <col min="2" max="2" width="52.85546875" style="15"/>
-    <col min="3" max="3" width="21" style="15"/>
-    <col min="4" max="4" width="20.85546875" style="15"/>
-    <col min="5" max="5" width="12.85546875" style="15"/>
-    <col min="6" max="6" width="11.28515625" style="15"/>
-    <col min="7" max="7" width="10.85546875" style="15"/>
-    <col min="8" max="8" width="23.42578125" style="15"/>
-    <col min="9" max="1025" width="11.5703125" style="15"/>
+    <col min="1" max="1" width="2.5703125" style="1"/>
+    <col min="2" max="2" width="52.85546875" style="1"/>
+    <col min="3" max="3" width="21" style="1"/>
+    <col min="4" max="4" width="20.85546875" style="1"/>
+    <col min="5" max="5" width="12.85546875" style="1"/>
+    <col min="6" max="6" width="11.28515625" style="1"/>
+    <col min="7" max="7" width="10.85546875" style="1"/>
+    <col min="8" max="8" width="23.42578125" style="1"/>
+    <col min="9" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024" ht="14.25" customHeight="1">
@@ -2272,12 +2281,12 @@
       <c r="AMJ1"/>
     </row>
     <row r="2" spans="1:1024" ht="15.75">
-      <c r="A2" s="16"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="A2" s="2"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
@@ -4325,13 +4334,13 @@
     </row>
     <row r="4" spans="1:1024" ht="16.5">
       <c r="A4"/>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="55"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
@@ -5353,13 +5362,15 @@
     </row>
     <row r="5" spans="1:1024" ht="13.9" customHeight="1">
       <c r="A5"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="C5" s="57" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
@@ -6381,13 +6392,15 @@
     </row>
     <row r="6" spans="1:1024" ht="12.75" customHeight="1">
       <c r="A6"/>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="C6" s="70">
+        <v>42468</v>
+      </c>
+      <c r="D6" s="57"/>
+      <c r="E6" s="57"/>
+      <c r="F6" s="57"/>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
@@ -7409,13 +7422,15 @@
     </row>
     <row r="7" spans="1:1024" ht="12.75" customHeight="1">
       <c r="A7"/>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="C7" s="57" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
@@ -11515,12 +11530,12 @@
     </row>
     <row r="11" spans="1:1024" ht="16.5" customHeight="1">
       <c r="A11"/>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="19"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="5"/>
       <c r="F11"/>
       <c r="G11"/>
       <c r="H11"/>
@@ -12543,13 +12558,13 @@
     </row>
     <row r="12" spans="1:1024" ht="16.5" customHeight="1">
       <c r="A12"/>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="C12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E12"/>
@@ -13575,14 +13590,14 @@
     </row>
     <row r="13" spans="1:1024" ht="16.5" customHeight="1">
       <c r="A13"/>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="9">
         <f>COUNTA(procesos!C3:C9)</f>
         <v>0</v>
       </c>
-      <c r="D13" s="24" t="e">
+      <c r="D13" s="10" t="e">
         <f>COUNTIF(procesos!C3:C9,"x")/(COUNTIF((procesos!C3:C9),"x")+COUNTIF((procesos!D3:D9),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -14609,14 +14624,14 @@
     </row>
     <row r="14" spans="1:1024" ht="16.5" customHeight="1">
       <c r="A14"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="9">
         <f>COUNTA(procesos!C26:C30)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="24" t="e">
+      <c r="D14" s="10" t="e">
         <f>COUNTIF(procesos!C26:C30,"x")/(COUNTIF((procesos!C26:C30),"x")+COUNTIF((procesos!D26:D30),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -15643,14 +15658,14 @@
     </row>
     <row r="15" spans="1:1024" ht="19.5" customHeight="1">
       <c r="A15"/>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="9">
         <f>COUNTA(procesos!C13:C17)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="24" t="e">
+      <c r="D15" s="10" t="e">
         <f>COUNTIF(procesos!C13:C17,"x")/(COUNTIF((procesos!C13:C17),"x")+COUNTIF((procesos!D13:D17),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -16675,91 +16690,91 @@
       <c r="AMI15"/>
       <c r="AMJ15"/>
     </row>
-    <row r="16" spans="1:1024" s="25" customFormat="1" ht="12.75"/>
-    <row r="17" spans="2:4" s="25" customFormat="1" ht="12.75"/>
+    <row r="16" spans="1:1024" s="11" customFormat="1" ht="12.75"/>
+    <row r="17" spans="2:4" s="11" customFormat="1" ht="12.75"/>
     <row r="18" spans="2:4" ht="16.5">
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="55"/>
+      <c r="D18" s="55"/>
     </row>
     <row r="19" spans="2:4">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="C19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:4">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="23">
+      <c r="C20" s="9">
         <f>COUNTA(Productos!C3:C7)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="24" t="e">
+      <c r="D20" s="10" t="e">
         <f>COUNTIF(Productos!C3:C7,"x")/(COUNTIF((Productos!C3:C7),"x")+COUNTIF((Productos!D3:D7),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="2:4">
-      <c r="B21" s="22" t="str">
+      <c r="B21" s="8" t="str">
         <f>Productos!A10</f>
         <v>Plan de Métricas</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="9">
         <f>COUNTA(Productos!C12:C19)</f>
         <v>0</v>
       </c>
-      <c r="D21" s="24" t="e">
+      <c r="D21" s="10" t="e">
         <f>COUNTIF(Productos!C12:C19,"x")/(COUNTIF((Productos!C12:C19),"x")+COUNTIF((Productos!D12:D19),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="2:4">
-      <c r="B22" s="22" t="str">
+      <c r="B22" s="8" t="str">
         <f>Productos!A22</f>
         <v>Plan de Configuración</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="9">
         <f>COUNTA(Productos!C24:C30)</f>
         <v>0</v>
       </c>
-      <c r="D22" s="24" t="e">
+      <c r="D22" s="10" t="e">
         <f>COUNTIF(Productos!C24:C30,"x")/(COUNTIF((Productos!C24:C30),"x")+COUNTIF((Productos!D24:D30),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="2:4">
-      <c r="B23" s="22" t="str">
+      <c r="B23" s="8" t="str">
         <f>Productos!A50</f>
         <v>Plan de proyecto</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="9">
         <f>COUNTA(Productos!C52:C70)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="24" t="e">
+      <c r="D23" s="10" t="e">
         <f>COUNTIF(Productos!C52:C70,"x")/(COUNTIF((Productos!C52:C70),"x")+COUNTIF((Productos!D52:D70),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="2:4">
-      <c r="B24" s="22" t="str">
+      <c r="B24" s="8" t="str">
         <f>Productos!A35</f>
         <v>Reporte de Monitoreo</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="9">
         <f>COUNTA(Productos!C37:C45)</f>
         <v>0</v>
       </c>
-      <c r="D24" s="24" t="e">
+      <c r="D24" s="10" t="e">
         <f>COUNTIF(Productos!C37:C45,"x")/(COUNTIF((Productos!C37:C45),"x")+COUNTIF((Productos!D37:D45),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -16775,33 +16790,33 @@
       <c r="D26"/>
     </row>
     <row r="27" spans="2:4" ht="16.5">
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
     </row>
     <row r="28" spans="2:4">
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" spans="2:4">
-      <c r="B29" s="22" t="str">
+      <c r="B29" s="8" t="str">
         <f>Funcional!A3</f>
         <v>Líneas Base</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="9">
         <f>COUNTA(Funcional!C4:C6)</f>
         <v>0</v>
       </c>
-      <c r="D29" s="24" t="e">
+      <c r="D29" s="10" t="e">
         <f>COUNTIF(Funcional!C4:C6,"x")/(COUNTIF((Funcional!C4:C6),"x")+COUNTIF((Funcional!D4:D6),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -16817,47 +16832,47 @@
       <c r="D31"/>
     </row>
     <row r="32" spans="2:4" ht="16.5">
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
+      <c r="C32" s="55"/>
+      <c r="D32" s="55"/>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="20" t="s">
+      <c r="B33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="2:4">
-      <c r="B34" s="22" t="str">
+      <c r="B34" s="8" t="str">
         <f>Física!A3</f>
         <v>Elementos de Configuración</v>
       </c>
-      <c r="C34" s="23">
+      <c r="C34" s="9">
         <f>COUNTA(Física!C4:C6)</f>
         <v>0</v>
       </c>
-      <c r="D34" s="24" t="e">
+      <c r="D34" s="10" t="e">
         <f>COUNTIF(Física!C4:C6,"x")/(COUNTIF((Física!C4:C6),"x")+COUNTIF((Física!D4:D6),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="35" spans="2:4">
-      <c r="B35" s="22" t="str">
+      <c r="B35" s="8" t="str">
         <f>Física!A7</f>
         <v>Línea Base</v>
       </c>
-      <c r="C35" s="23">
+      <c r="C35" s="9">
         <f>COUNTA(Física!C8:C11)</f>
         <v>0</v>
       </c>
-      <c r="D35" s="24" t="e">
+      <c r="D35" s="10" t="e">
         <f>COUNTIF(Física!C8:C11,"x")/(COUNTIF((Física!C8:C11),"x")+COUNTIF((Física!D8:D11),"x"))</f>
         <v>#DIV/0!</v>
       </c>
@@ -16873,91 +16888,91 @@
       <c r="D37"/>
     </row>
     <row r="38" spans="2:4" ht="16.5">
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="55"/>
     </row>
     <row r="39" spans="2:4">
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D39" s="21" t="s">
+      <c r="D39" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="40" spans="2:4">
-      <c r="B40" s="22" t="str">
+      <c r="B40" s="8" t="str">
         <f>'Monitoreo Actividades'!A3</f>
         <v>Actividades de ventas</v>
       </c>
-      <c r="C40" s="23">
+      <c r="C40" s="9">
         <f>COUNTA('Monitoreo Actividades'!C4:C7)</f>
         <v>2</v>
       </c>
-      <c r="D40" s="24">
+      <c r="D40" s="10">
         <f>COUNTIF('Monitoreo Actividades'!C4:C7,"x")/(COUNTIF(('Monitoreo Actividades'!C4:C7),"x")+COUNTIF(('Monitoreo Actividades'!D4:D7),"x"))</f>
         <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="2:4">
-      <c r="B41" s="22" t="str">
+      <c r="B41" s="8" t="str">
         <f>'Monitoreo Actividades'!A13</f>
         <v>Actividades de planeación anual</v>
       </c>
-      <c r="C41" s="23">
+      <c r="C41" s="9">
         <f>COUNTA('Monitoreo Actividades'!C14:C16)</f>
         <v>0</v>
       </c>
-      <c r="D41" s="24" t="e">
+      <c r="D41" s="10" t="e">
         <f>COUNTIF('Monitoreo Actividades'!C14:C16,"x")/(COUNTIF(('Monitoreo Actividades'!C14:C16),"x")+COUNTIF(('Monitoreo Actividades'!D14:D16),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="42" spans="2:4">
-      <c r="B42" s="22" t="str">
+      <c r="B42" s="8" t="str">
         <f>'Monitoreo Actividades'!A22</f>
         <v>Actividades Organizacional</v>
       </c>
-      <c r="C42" s="23">
+      <c r="C42" s="9">
         <f>COUNTA('Monitoreo Actividades'!C23:C25)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="24" t="e">
+      <c r="D42" s="10" t="e">
         <f>COUNTIF('Monitoreo Actividades'!C23:C25,"x")/(COUNTIF(('Monitoreo Actividades'!C23:C25),"x")+COUNTIF(('Monitoreo Actividades'!D23:D25),"x"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="43" spans="2:4">
-      <c r="B43" s="22" t="str">
+      <c r="B43" s="8" t="str">
         <f>'Monitoreo Actividades'!A32</f>
         <v>Actividades Compras</v>
       </c>
-      <c r="C43" s="23">
+      <c r="C43" s="9">
         <f>COUNTA('Monitoreo Actividades'!C33:C36)</f>
         <v>4</v>
       </c>
-      <c r="D43" s="24">
+      <c r="D43" s="10">
         <f>COUNTIF('Monitoreo Actividades'!C33:C36,"x")/(COUNTIF(('Monitoreo Actividades'!C33:C36),"x")+COUNTIF(('Monitoreo Actividades'!D33:D36),"x"))</f>
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="1.14375" bottom="1.14375" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -16982,370 +16997,370 @@
     <col min="1024" max="1025" width="10.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="27" customFormat="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:6" s="13" customFormat="1">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="58"/>
+      <c r="C1" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="9"/>
+      <c r="F2" s="60"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="30">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="31"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:6" s="27" customFormat="1">
-      <c r="A4" s="30">
+    <row r="4" spans="1:6" s="13" customFormat="1">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:6" s="27" customFormat="1">
-      <c r="A5" s="30">
+    <row r="5" spans="1:6" s="13" customFormat="1">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:6" s="27" customFormat="1">
-      <c r="A6" s="30">
+    <row r="6" spans="1:6" s="13" customFormat="1">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="31"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="1:6" s="27" customFormat="1">
-      <c r="A7" s="30">
+    <row r="7" spans="1:6" s="13" customFormat="1">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="17"/>
     </row>
-    <row r="8" spans="1:6" s="27" customFormat="1">
-      <c r="A8" s="30">
+    <row r="8" spans="1:6" s="13" customFormat="1">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="31"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="17"/>
     </row>
-    <row r="9" spans="1:6" s="27" customFormat="1">
-      <c r="A9" s="30">
+    <row r="9" spans="1:6" s="13" customFormat="1">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="31"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="58" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="58"/>
+      <c r="C11" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="9" t="s">
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="28" t="s">
+      <c r="A12" s="58"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="29" t="s">
+      <c r="E12" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="60"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="30">
+      <c r="A13" s="16">
         <v>1</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="30">
+      <c r="A14" s="16">
         <v>2</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="30">
+      <c r="A15" s="16">
         <v>3</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="30">
+      <c r="A16" s="16">
         <v>4</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="30">
+      <c r="A17" s="16">
         <v>5</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="10" t="s">
+      <c r="B24" s="58"/>
+      <c r="C24" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="9" t="s">
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="28" t="s">
+      <c r="A25" s="58"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="60"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="30">
+      <c r="A26" s="16">
         <v>1</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="30">
+      <c r="A27" s="16">
         <v>2</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="30">
+      <c r="A28" s="16">
         <v>3</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="30">
+      <c r="A29" s="16">
         <v>4</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="30">
+      <c r="A30" s="16">
         <v>5</v>
       </c>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="31"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="17"/>
     </row>
-    <row r="31" spans="1:6" s="27" customFormat="1"/>
-    <row r="32" spans="1:6" s="27" customFormat="1">
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
+    <row r="31" spans="1:6" s="13" customFormat="1"/>
+    <row r="32" spans="1:6" s="13" customFormat="1">
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="2:5" s="27" customFormat="1">
+    <row r="33" spans="2:5" s="13" customFormat="1">
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33"/>
     </row>
-    <row r="34" spans="2:5" s="27" customFormat="1">
+    <row r="34" spans="2:5" s="13" customFormat="1">
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34"/>
     </row>
-    <row r="35" spans="2:5" s="27" customFormat="1">
+    <row r="35" spans="2:5" s="13" customFormat="1">
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35"/>
     </row>
-    <row r="36" spans="2:5" s="27" customFormat="1">
+    <row r="36" spans="2:5" s="13" customFormat="1">
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36"/>
     </row>
-    <row r="37" spans="2:5" s="27" customFormat="1">
+    <row r="37" spans="2:5" s="13" customFormat="1">
       <c r="C37"/>
       <c r="D37"/>
       <c r="E37"/>
     </row>
-    <row r="38" spans="2:5" s="27" customFormat="1">
+    <row r="38" spans="2:5" s="13" customFormat="1">
       <c r="C38"/>
       <c r="D38"/>
       <c r="E38"/>
     </row>
-    <row r="39" spans="2:5" s="27" customFormat="1">
+    <row r="39" spans="2:5" s="13" customFormat="1">
       <c r="C39"/>
       <c r="D39"/>
       <c r="E39"/>
     </row>
-    <row r="40" spans="2:5" s="27" customFormat="1">
+    <row r="40" spans="2:5" s="13" customFormat="1">
       <c r="C40"/>
       <c r="D40"/>
       <c r="E40"/>
     </row>
-    <row r="41" spans="2:5" s="27" customFormat="1">
+    <row r="41" spans="2:5" s="13" customFormat="1">
       <c r="C41"/>
       <c r="D41"/>
       <c r="E41"/>
     </row>
-    <row r="42" spans="2:5" s="27" customFormat="1">
+    <row r="42" spans="2:5" s="13" customFormat="1">
       <c r="C42"/>
       <c r="D42"/>
       <c r="E42"/>
     </row>
-    <row r="43" spans="2:5" s="27" customFormat="1">
+    <row r="43" spans="2:5" s="13" customFormat="1">
       <c r="C43"/>
       <c r="D43"/>
       <c r="E43"/>
     </row>
-    <row r="44" spans="2:5" s="27" customFormat="1">
+    <row r="44" spans="2:5" s="13" customFormat="1">
       <c r="C44"/>
       <c r="D44"/>
       <c r="E44"/>
     </row>
-    <row r="45" spans="2:5" s="27" customFormat="1">
+    <row r="45" spans="2:5" s="13" customFormat="1">
       <c r="C45"/>
       <c r="D45"/>
       <c r="E45"/>
     </row>
-    <row r="46" spans="2:5" s="27" customFormat="1">
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
+    <row r="46" spans="2:5" s="13" customFormat="1">
+      <c r="B46" s="61"/>
+      <c r="C46" s="61"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -17383,737 +17398,743 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="10" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="6" t="s">
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="28" t="s">
+      <c r="A2" s="62"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="6"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:6" ht="18.75" customHeight="1">
-      <c r="A4" s="34">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="37"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="34">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="34">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="37"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="23"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="39">
+      <c r="A7" s="25">
         <v>5</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="37"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="33"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="58"/>
+      <c r="C10" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="9" t="s">
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="28" t="s">
+      <c r="A11" s="58"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="29" t="s">
+      <c r="D11" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="29" t="s">
+      <c r="E11" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="60"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="30">
+      <c r="A12" s="16">
         <v>1</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="31"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="30">
+      <c r="A13" s="16">
         <v>2</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="17"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="30">
+      <c r="A14" s="16">
         <v>3</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="31"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="17"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="30">
+      <c r="A15" s="16">
         <v>4</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="31"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="30">
+      <c r="A16" s="16">
         <v>5</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="31"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="30">
+      <c r="A17" s="16">
         <v>6</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="31"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="30">
+      <c r="A18" s="16">
         <v>7</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="31"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="30">
+      <c r="A19" s="16">
         <v>8</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="31"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="58"/>
+      <c r="C22" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="9" t="s">
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="28" t="s">
+      <c r="A23" s="58"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" s="60"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="30">
+      <c r="A24" s="16">
         <v>1</v>
       </c>
-      <c r="B24" s="31" t="s">
+      <c r="B24" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="31"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="30">
+      <c r="A25" s="16">
         <v>2</v>
       </c>
-      <c r="B25" s="41" t="s">
+      <c r="B25" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="30">
+      <c r="A26" s="16">
         <v>3</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="30">
+      <c r="A27" s="16">
         <v>4</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="31"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="30">
+      <c r="A28" s="16">
         <v>5</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="43">
+      <c r="A29" s="29">
         <v>7</v>
       </c>
-      <c r="B29" s="41" t="s">
+      <c r="B29" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="43">
+      <c r="A30" s="29">
         <v>8</v>
       </c>
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="B31" s="45"/>
+      <c r="B31" s="31"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="B32" s="45"/>
+      <c r="B32" s="31"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="10" t="s">
+      <c r="B35" s="58"/>
+      <c r="C35" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="9" t="s">
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="28" t="s">
+      <c r="A36" s="58"/>
+      <c r="B36" s="58"/>
+      <c r="C36" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="29" t="s">
+      <c r="D36" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="E36" s="29" t="s">
+      <c r="E36" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="9"/>
+      <c r="F36" s="60"/>
     </row>
     <row r="37" spans="1:6" ht="26.25">
-      <c r="A37" s="30">
+      <c r="A37" s="16">
         <v>1</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="30">
+      <c r="A38" s="16">
         <v>2</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="31"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="30">
+      <c r="A39" s="16">
         <v>3</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="31"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="30">
+      <c r="A40" s="16">
         <v>4</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="17"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="46">
+      <c r="A41" s="32">
         <v>5</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B41" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46"/>
-      <c r="F41" s="47"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="33"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="30">
+      <c r="A42" s="16">
         <v>6</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B42" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="43"/>
-      <c r="F42" s="44"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="30"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="30">
+      <c r="A43" s="16">
         <v>7</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B43" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="43"/>
-      <c r="D43" s="43"/>
-      <c r="E43" s="43"/>
-      <c r="F43" s="44"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="30"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="30">
+      <c r="A44" s="16">
         <v>8</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B44" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-      <c r="E44" s="43"/>
-      <c r="F44" s="44"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="30">
+      <c r="A45" s="16">
         <v>9</v>
       </c>
-      <c r="B45" s="42" t="s">
+      <c r="B45" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C45" s="43"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="43"/>
-      <c r="F45" s="44"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
     </row>
-    <row r="50" spans="1:6" s="48" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="11" t="s">
+    <row r="50" spans="1:6" s="34" customFormat="1" ht="15" customHeight="1">
+      <c r="A50" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="10" t="s">
+      <c r="B50" s="58"/>
+      <c r="C50" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="9" t="s">
+      <c r="D50" s="59"/>
+      <c r="E50" s="59"/>
+      <c r="F50" s="60" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="15" customHeight="1">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="26" t="s">
+      <c r="A51" s="58"/>
+      <c r="B51" s="58"/>
+      <c r="C51" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="D51" s="49" t="s">
+      <c r="D51" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E51" s="49" t="s">
+      <c r="E51" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F51" s="9"/>
+      <c r="F51" s="60"/>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="50">
+      <c r="A52" s="36">
         <v>1</v>
       </c>
-      <c r="B52" s="51" t="s">
+      <c r="B52" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="52"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="38"/>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="34">
+      <c r="A53" s="20">
         <v>2</v>
       </c>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="39" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="52"/>
+      <c r="C53" s="20"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="38"/>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="34">
+      <c r="A54" s="20">
         <v>3</v>
       </c>
-      <c r="B54" s="53" t="s">
+      <c r="B54" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="52"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="38"/>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="34">
+      <c r="A55" s="20">
         <v>4</v>
       </c>
-      <c r="B55" s="53" t="s">
+      <c r="B55" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="34"/>
-      <c r="F55" s="52"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="38"/>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="34">
+      <c r="A56" s="20">
         <v>6</v>
       </c>
-      <c r="B56" s="53" t="s">
+      <c r="B56" s="39" t="s">
         <v>76</v>
       </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="52"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="38"/>
     </row>
     <row r="57" spans="1:6" ht="30">
-      <c r="A57" s="34">
+      <c r="A57" s="20">
         <v>7</v>
       </c>
-      <c r="B57" s="54" t="s">
+      <c r="B57" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="52"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="38"/>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="34">
+      <c r="A58" s="20">
         <v>8</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B58" s="40" t="s">
         <v>78</v>
       </c>
-      <c r="C58" s="34"/>
-      <c r="D58" s="34"/>
-      <c r="E58" s="34"/>
-      <c r="F58" s="52"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="38"/>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="34">
+      <c r="A59" s="20">
         <v>9</v>
       </c>
-      <c r="B59" s="54" t="s">
+      <c r="B59" s="40" t="s">
         <v>79</v>
       </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="52"/>
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="38"/>
     </row>
     <row r="60" spans="1:6" ht="30">
-      <c r="A60" s="34">
+      <c r="A60" s="20">
         <v>10</v>
       </c>
-      <c r="B60" s="54" t="s">
+      <c r="B60" s="40" t="s">
         <v>80</v>
       </c>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="52"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="38"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="34">
+      <c r="A61" s="20">
         <v>11</v>
       </c>
-      <c r="B61" s="54" t="s">
+      <c r="B61" s="40" t="s">
         <v>81</v>
       </c>
-      <c r="C61" s="34"/>
-      <c r="D61" s="34"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="52"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="20"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="38"/>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="34">
+      <c r="A62" s="20">
         <v>12</v>
       </c>
-      <c r="B62" s="54" t="s">
+      <c r="B62" s="40" t="s">
         <v>82</v>
       </c>
-      <c r="C62" s="34"/>
-      <c r="D62" s="34"/>
-      <c r="E62" s="34"/>
-      <c r="F62" s="52"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="20"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="38"/>
     </row>
     <row r="63" spans="1:6" ht="30">
-      <c r="A63" s="34">
+      <c r="A63" s="20">
         <v>11</v>
       </c>
-      <c r="B63" s="54" t="s">
+      <c r="B63" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="52"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="38"/>
     </row>
     <row r="64" spans="1:6">
-      <c r="A64" s="34">
+      <c r="A64" s="20">
         <v>12</v>
       </c>
-      <c r="B64" s="53" t="s">
+      <c r="B64" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="C64" s="34"/>
-      <c r="D64" s="34"/>
-      <c r="E64" s="34"/>
-      <c r="F64" s="52"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="20"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="38"/>
     </row>
     <row r="65" spans="1:6">
-      <c r="A65" s="34">
+      <c r="A65" s="20">
         <v>13</v>
       </c>
-      <c r="B65" s="53" t="s">
+      <c r="B65" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="52"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="38"/>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="34">
+      <c r="A66" s="20">
         <v>14</v>
       </c>
-      <c r="B66" s="53" t="s">
+      <c r="B66" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C66" s="34"/>
-      <c r="D66" s="34"/>
-      <c r="E66" s="34"/>
-      <c r="F66" s="52"/>
+      <c r="C66" s="20"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="38"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="55">
+      <c r="A67" s="41">
         <v>15</v>
       </c>
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="34"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="52"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="38"/>
     </row>
     <row r="68" spans="1:6">
-      <c r="A68" s="34">
+      <c r="A68" s="20">
         <v>16</v>
       </c>
-      <c r="B68" s="57" t="s">
+      <c r="B68" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="44"/>
+      <c r="E68" s="44"/>
+      <c r="F68" s="44"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="A69" s="34">
+      <c r="A69" s="20">
         <v>17</v>
       </c>
-      <c r="B69" s="57" t="s">
+      <c r="B69" s="43" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="44"/>
     </row>
     <row r="70" spans="1:6">
-      <c r="A70" s="34">
+      <c r="A70" s="20">
         <v>18</v>
       </c>
-      <c r="B70" s="57" t="s">
+      <c r="B70" s="43" t="s">
         <v>90</v>
       </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="44"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A10:B11"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:F11"/>
     <mergeCell ref="A50:B51"/>
     <mergeCell ref="C50:E50"/>
     <mergeCell ref="F50:F51"/>
@@ -18123,12 +18144,6 @@
     <mergeCell ref="A35:B36"/>
     <mergeCell ref="C35:E35"/>
     <mergeCell ref="F35:F36"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A10:B11"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -18153,78 +18168,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="5"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="64"/>
+      <c r="B1" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.5">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="59" t="s">
+      <c r="A2" s="64"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" spans="1:6" ht="25.5">
-      <c r="A4" s="62">
+      <c r="A4" s="48">
         <v>1</v>
       </c>
-      <c r="B4" s="63" t="s">
+      <c r="B4" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="51"/>
     </row>
     <row r="5" spans="1:6" ht="25.5">
-      <c r="A5" s="62">
+      <c r="A5" s="48">
         <v>2</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="66"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:6" ht="25.5">
-      <c r="A6" s="62">
+      <c r="A6" s="48">
         <v>3</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="65"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -18257,136 +18272,136 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="31.5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="59" t="s">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="46"/>
     </row>
     <row r="4" spans="1:6" ht="26.25">
-      <c r="A4" s="62">
+      <c r="A4" s="48">
         <v>1</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="66"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" ht="26.25">
-      <c r="A5" s="62">
+      <c r="A5" s="48">
         <v>2</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="66"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="52"/>
     </row>
     <row r="6" spans="1:6" ht="26.25">
-      <c r="A6" s="62">
+      <c r="A6" s="48">
         <v>3</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="66"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="52"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="60"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="46"/>
     </row>
     <row r="8" spans="1:6" ht="26.25">
-      <c r="A8" s="62">
+      <c r="A8" s="48">
         <v>1</v>
       </c>
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="66"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="52"/>
     </row>
     <row r="9" spans="1:6" ht="26.25">
-      <c r="A9" s="62">
+      <c r="A9" s="48">
         <v>2</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="66"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="52"/>
     </row>
     <row r="10" spans="1:6" ht="26.25">
-      <c r="A10" s="62">
+      <c r="A10" s="48">
         <v>3</v>
       </c>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="66"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="52"/>
     </row>
     <row r="11" spans="1:6" ht="39">
-      <c r="A11" s="62">
+      <c r="A11" s="48">
         <v>4</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="64"/>
-      <c r="F11" s="66"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -18405,7 +18420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:E1"/>
     </sheetView>
   </sheetViews>
@@ -18416,42 +18431,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="31.5">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="59" t="s">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="67"/>
     </row>
     <row r="3" spans="1:9" ht="14.85" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="66" t="s">
         <v>108</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="60"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="46"/>
       <c r="G3" s="69" t="s">
         <v>109</v>
       </c>
@@ -18459,18 +18474,18 @@
       <c r="I3" s="69"/>
     </row>
     <row r="4" spans="1:9" ht="51">
-      <c r="A4" s="62">
+      <c r="A4" s="48">
         <v>1</v>
       </c>
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="53" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64" t="s">
+      <c r="C4" s="50"/>
+      <c r="D4" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="E4" s="64"/>
-      <c r="F4" s="66" t="s">
+      <c r="E4" s="50"/>
+      <c r="F4" s="52" t="s">
         <v>122</v>
       </c>
       <c r="G4" s="69"/>
@@ -18478,35 +18493,35 @@
       <c r="I4" s="69"/>
     </row>
     <row r="5" spans="1:9" ht="39">
-      <c r="A5" s="62">
+      <c r="A5" s="48">
         <v>2</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="64"/>
-      <c r="F5" s="66"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
       <c r="I5" s="69"/>
     </row>
     <row r="6" spans="1:9" ht="51">
-      <c r="A6" s="62">
+      <c r="A6" s="48">
         <v>3</v>
       </c>
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64" t="s">
+      <c r="C6" s="50"/>
+      <c r="D6" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="E6" s="64"/>
-      <c r="F6" s="66" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="52" t="s">
         <v>123</v>
       </c>
       <c r="G6" s="69"/>
@@ -18514,56 +18529,56 @@
       <c r="I6" s="69"/>
     </row>
     <row r="7" spans="1:9" ht="26.25">
-      <c r="A7" s="62">
+      <c r="A7" s="48">
         <v>4</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="66"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="52"/>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="68"/>
+      <c r="C11" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2" t="s">
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="31.5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="59" t="s">
+      <c r="A12" s="68"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="59" t="s">
+      <c r="D12" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E12" s="59" t="s">
+      <c r="E12" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="14.85" customHeight="1">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="60"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="46"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="46"/>
       <c r="G13" s="69" t="s">
         <v>115</v>
       </c>
@@ -18571,87 +18586,87 @@
       <c r="I13" s="69"/>
     </row>
     <row r="14" spans="1:9" ht="39">
-      <c r="A14" s="62">
+      <c r="A14" s="48">
         <v>1</v>
       </c>
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="66"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="52"/>
       <c r="G14" s="69"/>
       <c r="H14" s="69"/>
       <c r="I14" s="69"/>
     </row>
     <row r="15" spans="1:9" ht="26.25">
-      <c r="A15" s="62">
+      <c r="A15" s="48">
         <v>2</v>
       </c>
-      <c r="B15" s="67" t="s">
+      <c r="B15" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="64"/>
-      <c r="F15" s="66"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="52"/>
       <c r="G15" s="69"/>
       <c r="H15" s="69"/>
       <c r="I15" s="69"/>
     </row>
     <row r="16" spans="1:9" ht="26.25">
-      <c r="A16" s="62">
+      <c r="A16" s="48">
         <v>3</v>
       </c>
-      <c r="B16" s="67" t="s">
+      <c r="B16" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
-      <c r="F16" s="66"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="52"/>
       <c r="G16" s="69"/>
       <c r="H16" s="69"/>
       <c r="I16" s="69"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="68"/>
+      <c r="C20" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2" t="s">
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="31.5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="59" t="s">
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="59" t="s">
+      <c r="D21" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="E21" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F21" s="2"/>
+      <c r="F21" s="67"/>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="66" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="60"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="46"/>
       <c r="G22" s="69" t="s">
         <v>117</v>
       </c>
@@ -18659,87 +18674,87 @@
       <c r="I22" s="69"/>
     </row>
     <row r="23" spans="1:9" ht="39">
-      <c r="A23" s="62">
+      <c r="A23" s="48">
         <v>1</v>
       </c>
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
-      <c r="F23" s="66"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="52"/>
       <c r="G23" s="69"/>
       <c r="H23" s="69"/>
       <c r="I23" s="69"/>
     </row>
     <row r="24" spans="1:9" ht="26.25">
-      <c r="A24" s="62">
+      <c r="A24" s="48">
         <v>2</v>
       </c>
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="64"/>
-      <c r="D24" s="64"/>
-      <c r="E24" s="64"/>
-      <c r="F24" s="66"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="52"/>
       <c r="G24" s="69"/>
       <c r="H24" s="69"/>
       <c r="I24" s="69"/>
     </row>
     <row r="25" spans="1:9" ht="26.25">
-      <c r="A25" s="62">
+      <c r="A25" s="48">
         <v>3</v>
       </c>
-      <c r="B25" s="67" t="s">
+      <c r="B25" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="64"/>
-      <c r="F25" s="66"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="52"/>
       <c r="G25" s="69"/>
       <c r="H25" s="69"/>
       <c r="I25" s="69"/>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="3" t="s">
+      <c r="B30" s="68"/>
+      <c r="C30" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="2" t="s">
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="31.5">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="59" t="s">
+      <c r="A31" s="68"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="D31" s="59" t="s">
+      <c r="D31" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="67"/>
     </row>
     <row r="32" spans="1:9" ht="14.85" customHeight="1">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="66" t="s">
         <v>118</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="60"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="46"/>
       <c r="G32" s="69" t="s">
         <v>119</v>
       </c>
@@ -18747,92 +18762,92 @@
       <c r="I32" s="69"/>
     </row>
     <row r="33" spans="1:9" ht="39">
-      <c r="A33" s="62">
+      <c r="A33" s="48">
         <v>1</v>
       </c>
-      <c r="B33" s="67" t="s">
+      <c r="B33" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="64" t="s">
+      <c r="C33" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="66"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="52"/>
       <c r="G33" s="69"/>
       <c r="H33" s="69"/>
       <c r="I33" s="69"/>
     </row>
     <row r="34" spans="1:9" ht="26.25">
-      <c r="A34" s="62">
+      <c r="A34" s="48">
         <v>2</v>
       </c>
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="64" t="s">
+      <c r="C34" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="66"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="52"/>
       <c r="G34" s="69"/>
       <c r="H34" s="69"/>
       <c r="I34" s="69"/>
     </row>
     <row r="35" spans="1:9" ht="26.25">
-      <c r="A35" s="62">
+      <c r="A35" s="48">
         <v>3</v>
       </c>
-      <c r="B35" s="67" t="s">
+      <c r="B35" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="64" t="s">
+      <c r="C35" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="66"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="52"/>
       <c r="G35" s="69"/>
       <c r="H35" s="69"/>
       <c r="I35" s="69"/>
     </row>
     <row r="36" spans="1:9" ht="39">
-      <c r="A36" s="62">
+      <c r="A36" s="48">
         <v>3</v>
       </c>
-      <c r="B36" s="67" t="s">
+      <c r="B36" s="53" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="64" t="s">
+      <c r="C36" s="50" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="66"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:I6"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="G13:I16"/>
+    <mergeCell ref="A20:B21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="G22:I25"/>
     <mergeCell ref="A30:B31"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="F30:F31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="G32:I35"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="G22:I25"/>
-    <mergeCell ref="A11:B12"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G13:I16"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:I6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>